<commit_message>
updated version following written outline
</commit_message>
<xml_diff>
--- a/dummydata.xlsx
+++ b/dummydata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hillarytao/Documents/APP4WE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9412728-8F43-4542-A4BD-01D2BA53FB3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0DD2A2-3D2B-A34A-9D24-71AF4E9E4583}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16280" xr2:uid="{7BC293AF-8D7F-EC4C-9A58-CB39FB91D79D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Questions</t>
   </si>
@@ -60,6 +60,33 @@
   </si>
   <si>
     <t>P2</t>
+  </si>
+  <si>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>Q8</t>
+  </si>
+  <si>
+    <t>Q9</t>
+  </si>
+  <si>
+    <t>Q10</t>
+  </si>
+  <si>
+    <t>Q11</t>
+  </si>
+  <si>
+    <t>Q12</t>
+  </si>
+  <si>
+    <t>Q13</t>
+  </si>
+  <si>
+    <t>Q14</t>
+  </si>
+  <si>
+    <t>Q15</t>
   </si>
 </sst>
 </file>
@@ -411,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8113D2E-185B-2B48-B9A9-3E9BDEC4564A}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -435,10 +462,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -446,10 +473,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -457,10 +484,10 @@
         <v>3</v>
       </c>
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
         <v>3</v>
-      </c>
-      <c r="C4">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -471,7 +498,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -479,10 +506,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -490,9 +517,108 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
         <v>1</v>
       </c>
     </row>

</xml_diff>